<commit_message>
Report Screenshot dan Video
</commit_message>
<xml_diff>
--- a/Excel/B2B.xlsx
+++ b/Excel/B2B.xlsx
@@ -470,7 +470,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A90"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -600,9 +600,334 @@
         <v>5FZvCkHEHk</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>YsIgF2cHnN</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>RpPuTMRrFJ</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>PxYGyOXlue</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>T9Wv2Z21HX</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>xzvugZSjnu</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>O2XQE27noP</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>vBTO68XlLc</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>92NdKdDuI3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>KXWNFDQcAU</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Lv74x8QNgF</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>EgH1BXMdDt</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>syiS76rjYp</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>82b6G6ZTWp</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>HVSNS4kXHA</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>qz6C02DmUl</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>787ZL9LJDV</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>1aPf1qDOtn</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>O9EZI3m8qq</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>vFnRaZAJtp</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>IfCgdGe1H7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>w4qQieb4tQ</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>SVfas0iNyK</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>ri9yfS50Du</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>R8B4EZHsnV</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>OrZon85kC6</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>4aL5r6uq1N</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>k07l5vTt6g</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>QP1bTr7fYB</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>0zYI61h88z</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>8iV4KPBO2P</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>dnUUl9ywom</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>qGNqugSxOt</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Fy5iKPrAuY</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>0uSpYmRgO6</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>dJCIYuyY0r</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>YXUQn7gJcB</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>IpzsfX8eOq</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>6pNRFcNwxu</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Aaw9I1L4ig</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>wyMLuBf7iO</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>TDAirExIr1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>NrhPXZJ1Fi</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>JaAWp73dve</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>3O5VxPDjtl</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>y6ZJJm764k</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>YbLavVR7mV</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>PjZ8C0jHym</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>j6JA2UK2cL</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>V2uirQgFW2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>aVT79aSw7b</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>7wPuUBbQVd</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>QBhqOPAgmc</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>K2H9nFYon4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>ilk76xav59</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>KE0v7gCFJZ</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>ldfTAOYBFq</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>wFMxzgPukX</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>b9hvcO02eP</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>KpNXOENfsB</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>1mMSths9W4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>7aEDQTJb58</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>kS3Bn2kx6u</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>2fKKWhfFCv</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>mOmT4UJzHX</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>97MUUlFJJZ</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A90"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update edit dan hapus hooks.js
</commit_message>
<xml_diff>
--- a/Excel/B2B.xlsx
+++ b/Excel/B2B.xlsx
@@ -470,7 +470,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A90"/>
+  <dimension ref="A1:A93"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -925,9 +925,24 @@
         <v>97MUUlFJJZ</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>oq7XiX5LVt</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>eTGkZta5kR</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>VqRxXMuFgd</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A90"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A93"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
running dengan crud berbeda 1 x jalan browser berbarengan
</commit_message>
<xml_diff>
--- a/Excel/B2B.xlsx
+++ b/Excel/B2B.xlsx
@@ -472,7 +472,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A104"/>
+  <dimension ref="A1:A106"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -997,10 +997,19 @@
         <v>KKdOOr29gb</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>30VQmLjkKU</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>Fs18cQJDnU</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A104"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A106"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1038,7 +1047,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1048,9 +1057,24 @@
         <v>gn</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>KE</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Pt</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>jX</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Neg dan Positive sesuai Excel
</commit_message>
<xml_diff>
--- a/Excel/B2B.xlsx
+++ b/Excel/B2B.xlsx
@@ -418,8 +418,8 @@
       <c r="A2" t="str">
         <v>kurniaremon@gmail.com</v>
       </c>
-      <c r="B2">
-        <v>12345</v>
+      <c r="B2" t="str">
+        <v>Padang123</v>
       </c>
     </row>
   </sheetData>
@@ -456,7 +456,7 @@
         <v>PLAYWRIGHT_CUCUMBER7</v>
       </c>
       <c r="B2" t="str">
-        <v>#ffffff</v>
+        <v>#170101</v>
       </c>
       <c r="C2" t="str">
         <v>test123</v>
@@ -472,7 +472,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A106"/>
+  <dimension ref="A1:A115"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1007,9 +1007,54 @@
         <v>Fs18cQJDnU</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>Zv7rFuuzGN</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>0KbymM3g4f</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>utraHQup0f</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>zDqhQbgN0j</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>DOoi8yNV0b</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>zyotYaM1eN</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>Z0JgJdJUzwxz1u6mmKjwt9OwUEBTTwhrzVZPZ2JZaBLhUfOZPfBH5lAuqEXrSl2Z1F67fcierFSFloQteSjUhM4NllRlyYthyjh9OcLZSSnzT5rIb33JfXPYrP6BiyAyXdY9A26l0st8ZrUhxWetvWsZn7qlRsWsocEqKKipwQVrabMuddgZPm8FjVPFWWRWAsvGQ7fm1mbps1rBhVNQZxSTeqFwL2ZHpLbgZMPazrJFOT7B9ombQ4pNEJIbjjIxHvnFzHEk89BQXkOXVXKEK8apWDJNDCLVw0hGMXzw8zwM</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>Y4eo58PXf54H81wPWbVFLJfssb3gPatGBIk7yAwL55FIrCKWEVMyHHe5lGwcrLJrocENEErLZJo9LnPaM4vtEGwKhl4WPGcbMM1xQ752WPmwEZ7sPnS82VAgBIURNUKBDZaAtEA9pnFBANd3JyIEDeinvdvSYJ872Z6pePcVbAMV4OdwyHVqjmpPpbQVDzEDBaobV2rOyNrKhB50AE6ZdwFW1vr6v9USBJwUc227IR99qOyZYadRythNCl3s1H6fSLDFtBVeQPorDciKHJ8s5rCQChhXYhIyKDVgiWTg1tPN</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>9557487046</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A106"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A115"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1047,7 +1092,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1072,9 +1117,15 @@
         <v>jX</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>7N</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Neg dan Positive sesuai Excel part 2
</commit_message>
<xml_diff>
--- a/Excel/B2B.xlsx
+++ b/Excel/B2B.xlsx
@@ -472,7 +472,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A115"/>
+  <dimension ref="A1:A178"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1052,9 +1052,324 @@
         <v>9557487046</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>Qo4RAiS8U9Wm2EvUphMCHYACUQjJuG2AJabHvVO5q7eXEEusfgeEKzm2KfNePc8aFbaQN8b96dtVqurhvKtQm67ftqKYtFZDreZsnuywwzkiQqV4SNwi7gkPsAqjFiysFoctLkIPrYijA7H9Dv7G1JQzRMHKTCWvAbK0zEICk3KVMFpEfEIO9NTcNArbr8xhaMjkfcdXsd7PFfYAHLvIRLWHedXJFLIQo49gVQrB4yP8c7BCSirio4W2TiDEKbkiEyb3dsPRGxrgD6oSyaOVn8Mh45L6GPcK0AIme6keOhsU</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>DolpROR2Qb</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>u8f1idxWfg</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>0147244574</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>1966987359</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>6579312241</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>3374975490</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>4492887231</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>5551784754</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>0433408105</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>zKJYg2aa4lBHFJfaSfGUbKaYe5cFYpXXpXG3MgEj7zmEwSr2bZ1QpnacctJx8DyOlFaOkUlw4D8uqSiq4ERjV5FpI0inImJn4dn3Bj9gk14W9bixxViciMeVKlft4wmTFyUGvqV6xHZ0Tn25FazD1CmDO7SnaUKEgA8hIwvMSlBSn6trTy1Q9zRuFFC02XxKbyPa0Phn6bnuFjXCwZtI6Iv5XjnrNsxmSR301tA77VO97d6omxLH245OW1IY12kgONJwHSldKBtnF5Ntrq7TtMymyZQT5voy1y2tyS1pjeSR</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>lnDJJdwKFB</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>48phmMDiCv</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>2933203647</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>3822511343</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>4997728180</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>3959652755</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>9634620144</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>3799616821</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>5101502046</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>I1XPpFCh2k</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>W5VROSvOrXLmv2VUgGgrMWmTx6wcnOchf4Z8sXcmIS3c5XIyGwSSw3PhLhD2hAANp0kVrrOutyf7gEWWbDu8kmIWb5DFF5GR5sSPCrVHWj8nIeIe52qGRwjURap0qxm46PHG2YRUXDGE3lNU9ZfYvkqGRRkUekZ4wVMT2MxG0kP6MkeYVHdBRNZYpvsGokIUc1QSna3Jk59S6JNPuHCRBhRaL8BzkdCDJa8jYHYt4HHOeRPbB1MIoOQMbDXMO9DeqDCewwa2WkLH6eetf9ciKabkvvvHK2coxaZdscBfitap</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>X6WHRdIz0J</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>E841l5d9z2</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>3UwcbercQg</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>1880867142</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>5747371831</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>6096401041</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>2230971876</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>9384541231</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>9669953575</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>4878908071</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>VePsajuc76</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>jRNSHlqGf4WqjSJ09PfDxrVyqfk5afVJMsbZa00THCrdwP8zPZnR5Boe8OuG4rcI4peiXQWWW6Lgg2r8IJ2eSw7gXoq2siJKjRkTFluMpyCIP9ygnlUkZPVnwa3CByjeYL7BrWQhx2KgTVJ3fPS672ZUkqt8mOz2n0EPbzdj503xdKSSLrDvlHahqEneUcqdtxuQXMnN642np1gKgDeuOBOZK0gHZ9tVB8OKxqDaakLchvNe6TrhAwnivIzddpj9nNh5N6tSbz70xjiX61KDhUT4RUuMKEhC7qrF48fEB9Nu</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>azSu88glJs</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>VUB9j1m4w4</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>9150645582</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>6815456300</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>9377205548</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>5601056513</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>6410820580</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>pF6mk8qBiC</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>DyxwzQFTHcCaWLMFfg0dpEk83eb8863staUJbWt6dUwtRZNSWRSZe1OiW1EKcFfjbiylAgmm3VRDKXTU16qjG3B01TEBeHgt53IL3xRD98yzlKlqz27tOQQyeA6qbWf74DIiqZnyhW2ewvQBTF2SOsfrJXZ1xYFtBwhcXbyoE1TeUFNnrDdKrqRwFcgXWUgOi3ijK1OoioqWdCEcXP78QMgoqfulbjQacbGPpYw9hQmtOgpc3D6Q3wwMnBWuL509Liej3i2cS30nsAhHFHje4aRm7ogy85eO6zKj3g8fgBKy</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>DR5N1uCt6z</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>AdiLca6C2Q</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>6337675431</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>0670340895</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>5976723740</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>1276630955</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>2856235206</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>b53vffYR9y</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>4MUUd8nEoLaB0keYkzvEAMi2BUYK5fWZNyufmJpF7jhN3ef7FWtcQMfsxDpxLynjciy6WLLeUTw5aMYCnAzmpsH1YZYpPUm8rNSk3epBqrDHDwGPgFDcVzwJc8yiGUnwphIIUI8AirNsWPKmOhjh6tUJcPpx1M85snb584BWki5EHAaTZWKUhfsoCn9L0VXu3FwEXj0y8qamPvrUkQNMrJp42sbSCNbHWsFhtCzyektu61qXVgyASBxD9TuP9c5wGDiB4DV9QArYXL9eegnGFFNoWziQB6vLzf2Vvmwtc8l0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>vAhQbcpF5K</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>3EG8zfuNuZ</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>1290296475</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>4657258690</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>9453193043</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>5010755775</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>0692913884</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>6576562097</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>8629946208</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>qfEOjTuGMN</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>M1H2ACnJbO</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A115"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A178"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>